<commit_message>
Actualización plan de inversión
</commit_message>
<xml_diff>
--- a/static/documentos/formato_informe.xlsx
+++ b/static/documentos/formato_informe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dandr\PycharmProjects\sion\static\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pytho\PycharmProjects\sion\static\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B6F1DF-150E-4D90-B619-2B242C3E64E4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7A45C1-8733-4785-95E7-F63E13A9F708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -67,18 +67,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF025930"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -184,6 +178,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -192,51 +231,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -275,16 +269,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1428749</xdr:colOff>
+      <xdr:colOff>1438275</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AA6B743-9DDC-40BB-A0DC-6CE1294D2F84}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD917D22-DE5F-4C06-A67A-7DF3B739B973}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -307,7 +301,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1428749" cy="1428749"/>
+          <a:ext cx="1438275" cy="1438275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -620,7 +614,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:AZ4"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,113 +624,113 @@
   <sheetData>
     <row r="1" spans="1:52" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="8"/>
-      <c r="AT1" s="8"/>
-      <c r="AU1" s="8"/>
-      <c r="AV1" s="8"/>
-      <c r="AW1" s="8"/>
-      <c r="AX1" s="8"/>
-      <c r="AY1" s="8"/>
-      <c r="AZ1" s="9"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="12"/>
     </row>
     <row r="2" spans="1:52" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="11"/>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="11"/>
-      <c r="AQ2" s="11"/>
-      <c r="AR2" s="11"/>
-      <c r="AS2" s="11"/>
-      <c r="AT2" s="11"/>
-      <c r="AU2" s="11"/>
-      <c r="AV2" s="11"/>
-      <c r="AW2" s="11"/>
-      <c r="AX2" s="11"/>
-      <c r="AY2" s="11"/>
-      <c r="AZ2" s="12"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="9"/>
     </row>
     <row r="3" spans="1:52" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -850,277 +844,277 @@
     </row>
     <row r="5" spans="1:52" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="20"/>
-      <c r="AD5" s="20"/>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="20"/>
-      <c r="AI5" s="20"/>
-      <c r="AJ5" s="20"/>
-      <c r="AK5" s="20"/>
-      <c r="AL5" s="20"/>
-      <c r="AM5" s="20"/>
-      <c r="AN5" s="20"/>
-      <c r="AO5" s="20"/>
-      <c r="AP5" s="20"/>
-      <c r="AQ5" s="20"/>
-      <c r="AR5" s="20"/>
-      <c r="AS5" s="20"/>
-      <c r="AT5" s="20"/>
-      <c r="AU5" s="20"/>
-      <c r="AV5" s="20"/>
-      <c r="AW5" s="20"/>
-      <c r="AX5" s="20"/>
-      <c r="AY5" s="20"/>
-      <c r="AZ5" s="21"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="5"/>
+      <c r="AZ5" s="6"/>
     </row>
     <row r="6" spans="1:52" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="11"/>
-      <c r="AJ6" s="11"/>
-      <c r="AK6" s="11"/>
-      <c r="AL6" s="11"/>
-      <c r="AM6" s="11"/>
-      <c r="AN6" s="11"/>
-      <c r="AO6" s="11"/>
-      <c r="AP6" s="11"/>
-      <c r="AQ6" s="11"/>
-      <c r="AR6" s="11"/>
-      <c r="AS6" s="11"/>
-      <c r="AT6" s="11"/>
-      <c r="AU6" s="11"/>
-      <c r="AV6" s="11"/>
-      <c r="AW6" s="11"/>
-      <c r="AX6" s="11"/>
-      <c r="AY6" s="11"/>
-      <c r="AZ6" s="12"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="8"/>
+      <c r="AQ6" s="8"/>
+      <c r="AR6" s="8"/>
+      <c r="AS6" s="8"/>
+      <c r="AT6" s="8"/>
+      <c r="AU6" s="8"/>
+      <c r="AV6" s="8"/>
+      <c r="AW6" s="8"/>
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="9"/>
     </row>
     <row r="7" spans="1:52" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="20"/>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="20"/>
-      <c r="AC7" s="20"/>
-      <c r="AD7" s="20"/>
-      <c r="AE7" s="20"/>
-      <c r="AF7" s="20"/>
-      <c r="AG7" s="20"/>
-      <c r="AH7" s="20"/>
-      <c r="AI7" s="20"/>
-      <c r="AJ7" s="20"/>
-      <c r="AK7" s="20"/>
-      <c r="AL7" s="20"/>
-      <c r="AM7" s="20"/>
-      <c r="AN7" s="20"/>
-      <c r="AO7" s="20"/>
-      <c r="AP7" s="20"/>
-      <c r="AQ7" s="20"/>
-      <c r="AR7" s="20"/>
-      <c r="AS7" s="20"/>
-      <c r="AT7" s="20"/>
-      <c r="AU7" s="20"/>
-      <c r="AV7" s="20"/>
-      <c r="AW7" s="20"/>
-      <c r="AX7" s="20"/>
-      <c r="AY7" s="20"/>
-      <c r="AZ7" s="21"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="5"/>
+      <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
+      <c r="AW7" s="5"/>
+      <c r="AX7" s="5"/>
+      <c r="AY7" s="5"/>
+      <c r="AZ7" s="6"/>
     </row>
     <row r="8" spans="1:52" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="11"/>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="11"/>
-      <c r="AK8" s="11"/>
-      <c r="AL8" s="11"/>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="11"/>
-      <c r="AO8" s="11"/>
-      <c r="AP8" s="11"/>
-      <c r="AQ8" s="11"/>
-      <c r="AR8" s="11"/>
-      <c r="AS8" s="11"/>
-      <c r="AT8" s="11"/>
-      <c r="AU8" s="11"/>
-      <c r="AV8" s="11"/>
-      <c r="AW8" s="11"/>
-      <c r="AX8" s="11"/>
-      <c r="AY8" s="11"/>
-      <c r="AZ8" s="12"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="8"/>
+      <c r="AR8" s="8"/>
+      <c r="AS8" s="8"/>
+      <c r="AT8" s="8"/>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="8"/>
+      <c r="AW8" s="8"/>
+      <c r="AX8" s="8"/>
+      <c r="AY8" s="8"/>
+      <c r="AZ8" s="9"/>
     </row>
     <row r="9" spans="1:52" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-      <c r="AG9" s="5"/>
-      <c r="AH9" s="5"/>
-      <c r="AI9" s="5"/>
-      <c r="AJ9" s="5"/>
-      <c r="AK9" s="5"/>
-      <c r="AL9" s="5"/>
-      <c r="AM9" s="5"/>
-      <c r="AN9" s="5"/>
-      <c r="AO9" s="5"/>
-      <c r="AP9" s="5"/>
-      <c r="AQ9" s="5"/>
-      <c r="AR9" s="5"/>
-      <c r="AS9" s="5"/>
-      <c r="AT9" s="5"/>
-      <c r="AU9" s="5"/>
-      <c r="AV9" s="5"/>
-      <c r="AW9" s="5"/>
-      <c r="AX9" s="5"/>
-      <c r="AY9" s="5"/>
-      <c r="AZ9" s="5"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="21"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
+      <c r="AI9" s="20"/>
+      <c r="AJ9" s="20"/>
+      <c r="AK9" s="20"/>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="20"/>
+      <c r="AN9" s="20"/>
+      <c r="AO9" s="20"/>
+      <c r="AP9" s="20"/>
+      <c r="AQ9" s="20"/>
+      <c r="AR9" s="20"/>
+      <c r="AS9" s="20"/>
+      <c r="AT9" s="20"/>
+      <c r="AU9" s="20"/>
+      <c r="AV9" s="20"/>
+      <c r="AW9" s="20"/>
+      <c r="AX9" s="20"/>
+      <c r="AY9" s="20"/>
+      <c r="AZ9" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>